<commit_message>
acertando a validação de entradas
</commit_message>
<xml_diff>
--- a/Tabela de Pessoas.xlsx
+++ b/Tabela de Pessoas.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2025,6 +2025,555 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>joão P Santos</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>11912345678</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>25</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>43</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>joão P Santos</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>11912345678</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>25</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>43</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>asdasdasdasdasdasd</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>11912345678</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>25</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>43</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>joão P Santos</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>11912345678</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>25</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>43</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Joao de souza cruz</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1961226556</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>25</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>43</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>joão P Santos</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1191234567</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>25</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>43</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>joão P Santos</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1191234567</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>25</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>43</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>joão P Santos</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>11912345678</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>25</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>43</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>joão P Santos</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>11123456789</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>25</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>dsdh@gmm.com.br</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>06666000</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Mario Veloso Serqueira</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>43</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Carlos Drummord Andrade</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Caracas</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>